<commit_message>
Improve the Oldfield plots.
</commit_message>
<xml_diff>
--- a/data/Oldfield2014.xlsx
+++ b/data/Oldfield2014.xlsx
@@ -113,7 +113,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -401,11 +401,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2043465896"/>
-        <c:axId val="2043472568"/>
+        <c:axId val="-2125526520"/>
+        <c:axId val="-2125541448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2043465896"/>
+        <c:axId val="-2125526520"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -436,12 +436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043472568"/>
+        <c:crossAx val="-2125541448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2043472568"/>
+        <c:axId val="-2125541448"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -452,10 +452,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -489,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043465896"/>
+        <c:crossAx val="-2125526520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
@@ -823,11 +823,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2143760408"/>
-        <c:axId val="-2143754840"/>
+        <c:axId val="-2125911048"/>
+        <c:axId val="-2125905464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2143760408"/>
+        <c:axId val="-2125911048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32768.0"/>
@@ -858,13 +858,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143754840"/>
+        <c:crossAx val="-2125905464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8192.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143754840"/>
+        <c:axId val="-2125905464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500.0"/>
@@ -877,7 +877,7 @@
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -906,7 +906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143760408"/>
+        <c:crossAx val="-2125911048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1180,11 +1180,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2143707544"/>
-        <c:axId val="-2143702024"/>
+        <c:axId val="-2125857096"/>
+        <c:axId val="-2125851560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2143707544"/>
+        <c:axId val="-2125857096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32768.0"/>
@@ -1215,13 +1215,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143702024"/>
+        <c:crossAx val="-2125851560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8192.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143702024"/>
+        <c:axId val="-2125851560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1230,10 +1230,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="3175" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
@@ -1262,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143707544"/>
+        <c:crossAx val="-2125857096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2030,18 +2030,52 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office Classic">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Arial"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hang" typeface="돋움"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Times New Roman"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐ明朝"/>
+        <a:font script="Hang" typeface="바탕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -2064,42 +2098,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2320,7 +2318,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="5" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2464,7 +2462,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
@@ -2648,7 +2646,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>

</xml_diff>